<commit_message>
Updated file order.  Preparing for final analysis.
</commit_message>
<xml_diff>
--- a/Code/Results/6_jointAssociations.xlsx
+++ b/Code/Results/6_jointAssociations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4602" uniqueCount="4602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5601" uniqueCount="5601">
   <si>
     <t>outcomeVar</t>
   </si>
@@ -13820,6 +13820,3003 @@
   </si>
   <si>
     <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>glucose120</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>glucose120</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>glucose120</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>leptin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>mbpsys</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>mbpdia</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>nefa</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>ldl</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>hdl</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>hdl</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>cmrs</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>cmrs</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>cmrs</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>cmrs</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>glucose0</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>outcomeVar</t>
+  </si>
+  <si>
+    <t>Count: Women</t>
+  </si>
+  <si>
+    <t>Count: Men</t>
+  </si>
+  <si>
+    <t>Pvalue: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>AIC: base totalPAEE model</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model main effects</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model totalPAEE interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>AIC: cosinor model sex interactions</t>
+  </si>
+  <si>
+    <t>Pvalue: full cosinor model vs base totalPAEE model</t>
+  </si>
+  <si>
+    <t>glucose120</t>
   </si>
 </sst>
 </file>
@@ -13868,81 +16865,81 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4577</v>
+        <v>5576</v>
       </c>
       <c r="B1" t="s">
-        <v>4578</v>
+        <v>5577</v>
       </c>
       <c r="C1" t="s">
-        <v>4579</v>
+        <v>5578</v>
       </c>
       <c r="D1" t="s">
-        <v>4580</v>
+        <v>5579</v>
       </c>
       <c r="E1" t="s">
-        <v>4581</v>
+        <v>5580</v>
       </c>
       <c r="F1" t="s">
-        <v>4582</v>
+        <v>5581</v>
       </c>
       <c r="G1" t="s">
-        <v>4583</v>
+        <v>5582</v>
       </c>
       <c r="H1" t="s">
-        <v>4584</v>
+        <v>5583</v>
       </c>
       <c r="I1" t="s">
-        <v>4585</v>
+        <v>5584</v>
       </c>
       <c r="J1" t="s">
-        <v>4586</v>
+        <v>5585</v>
       </c>
       <c r="K1" t="s">
-        <v>4587</v>
+        <v>5586</v>
       </c>
       <c r="L1" t="s">
-        <v>4588</v>
+        <v>5587</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4601</v>
+        <v>5600</v>
       </c>
       <c r="B2">
-        <v>5160</v>
+        <v>6264</v>
       </c>
       <c r="C2">
-        <v>4496</v>
+        <v>5526</v>
       </c>
       <c r="D2">
-        <v>2.256083031230306e-25</v>
+        <v>1.236506681742469e-41</v>
       </c>
       <c r="E2">
-        <v>96490.52969322307</v>
+        <v>44228.80915806572</v>
       </c>
       <c r="F2">
-        <v>8.4422154900672097e-68</v>
+        <v>7.6239494739240742e-37</v>
       </c>
       <c r="G2">
-        <v>96168.560773518053</v>
+        <v>44053.310141253474</v>
       </c>
       <c r="H2">
-        <v>0.030115885031210883</v>
+        <v>0.13404121063276411</v>
       </c>
       <c r="I2">
-        <v>96168.092745431582</v>
+        <v>44057.626736596969</v>
       </c>
       <c r="J2">
-        <v>0.0041672434941977358</v>
+        <v>0.0012744926274930774</v>
       </c>
       <c r="K2">
-        <v>96162.006645113783</v>
+        <v>44048.382753221376</v>
       </c>
       <c r="L2">
-        <v>1.6103742779020925e-96</v>
+        <v>4.8776225638079059e-33</v>
       </c>
       <c r="M2">
-        <v>96102.187656800015</v>
+        <v>44051.06115482068</v>
       </c>
     </row>
     <row r="3">
@@ -14325,40 +17322,40 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>4589</v>
+        <v>5588</v>
       </c>
       <c r="B1" t="s">
-        <v>4590</v>
+        <v>5589</v>
       </c>
       <c r="C1" t="s">
-        <v>4591</v>
+        <v>5590</v>
       </c>
       <c r="D1" t="s">
-        <v>4592</v>
+        <v>5591</v>
       </c>
       <c r="E1" t="s">
-        <v>4593</v>
+        <v>5592</v>
       </c>
       <c r="F1" t="s">
-        <v>4594</v>
+        <v>5593</v>
       </c>
       <c r="G1" t="s">
-        <v>4595</v>
+        <v>5594</v>
       </c>
       <c r="H1" t="s">
-        <v>4596</v>
+        <v>5595</v>
       </c>
       <c r="I1" t="s">
-        <v>4597</v>
+        <v>5596</v>
       </c>
       <c r="J1" t="s">
-        <v>4598</v>
+        <v>5597</v>
       </c>
       <c r="K1" t="s">
-        <v>4599</v>
+        <v>5598</v>
       </c>
       <c r="L1" t="s">
-        <v>4600</v>
+        <v>5599</v>
       </c>
     </row>
     <row r="2">

</xml_diff>